<commit_message>
Der Klasse 'Nutzer' wurden alle Methoden zugefuegt, um alle vorhandenen Stored Procedures ansprechen zu koennen. Alle Methoden laufen wie erwartet.
</commit_message>
<xml_diff>
--- a/src/main/insert Entgeltdaten/3 Verguetungsbestandteil.xlsx
+++ b/src/main/insert Entgeltdaten/3 Verguetungsbestandteil.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\insert Entgeltdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C07D2FF-4BF0-4124-A6C3-AF51833DB37D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C4BAF4-F397-4610-9C88-03B79AFE4060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="1008" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -426,7 +426,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
SP fuer Verguetungsbestandteilgeschrieben. Unittests angepasst. Alle Tests laufen.
</commit_message>
<xml_diff>
--- a/src/main/insert Entgeltdaten/3 Verguetungsbestandteil.xlsx
+++ b/src/main/insert Entgeltdaten/3 Verguetungsbestandteil.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\insert Entgeltdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C4BAF4-F397-4610-9C88-03B79AFE4060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{842BCBB8-10A3-4D4A-B587-271E4DDE42BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33945" yWindow="3360" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Daten</t>
   </si>
@@ -80,21 +80,6 @@
   </si>
   <si>
     <t>Grundgehalt</t>
-  </si>
-  <si>
-    <t>Tarifbezeichnung</t>
-  </si>
-  <si>
-    <t>A5-1</t>
-  </si>
-  <si>
-    <t>Betrag</t>
-  </si>
-  <si>
-    <t>gueltig ab:</t>
-  </si>
-  <si>
-    <t>01.05.2023</t>
   </si>
 </sst>
 </file>
@@ -138,11 +123,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -423,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -457,30 +441,6 @@
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="3">
-        <v>3330.18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>